<commit_message>
docs: update access control flow for resource
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyicui/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VIRUS/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31B97AF3-A885-CE48-B083-B4AA1BFA143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587D0BEE-37B0-314B-A10A-9876AF76868A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
@@ -23,11 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>DELETE 1</t>
   </si>
@@ -80,6 +76,9 @@
   </si>
   <si>
     <t>TAG</t>
+  </si>
+  <si>
+    <t>RESOURCE</t>
   </si>
 </sst>
 </file>
@@ -187,12 +186,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB183B-02B6-F140-9F88-75932E878015}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,45 +556,45 @@
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="6"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="6"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -633,50 +632,127 @@
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="6"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B12:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
feat: add subscription model with api
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VIRUS/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587D0BEE-37B0-314B-A10A-9876AF76868A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BF4232-82D4-3248-A5A6-DFB17DA445C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
   <si>
     <t>DELETE 1</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>RESOURCE</t>
+  </si>
+  <si>
+    <t>SUBSCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -506,14 +509,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB183B-02B6-F140-9F88-75932E878015}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -748,11 +752,88 @@
       <c r="I14" s="7"/>
       <c r="J14" s="5"/>
     </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
add school model with api
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VIRUS/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66BF4232-82D4-3248-A5A6-DFB17DA445C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D11004D-BC3D-264C-A674-0767A1461B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
+    <workbookView xWindow="5960" yWindow="1820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="18">
   <si>
     <t>DELETE 1</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>SUBSCRIPTION</t>
+  </si>
+  <si>
+    <t>SCHOOL</t>
   </si>
 </sst>
 </file>
@@ -509,11 +512,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB183B-02B6-F140-9F88-75932E878015}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -715,7 +716,7 @@
       <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
@@ -791,9 +792,9 @@
       <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
       <c r="F17" s="5"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -828,12 +829,89 @@
       <c r="I19" s="7"/>
       <c r="J19" s="5"/>
     </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
update access control flow chart for subscription
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VIRUS/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D11004D-BC3D-264C-A674-0767A1461B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB087EA-6769-F149-B2BE-DCBFFB23FE06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="1820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
@@ -793,8 +793,8 @@
         <v>16</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>

</xml_diff>

<commit_message>
add recently visited model
- add XOR validator on resourceId and subscriptionId of recently visited
- add method to retrieve recently visited of given userId
- add queue data structure of size 6 when creating recently visited
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VIRUS/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonqiu/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB087EA-6769-F149-B2BE-DCBFFB23FE06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56F5181-AEB4-9E42-9E22-B41AEAED37B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="1820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
+    <workbookView xWindow="2200" yWindow="1820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
   <si>
     <t>DELETE 1</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>SCHOOL</t>
+  </si>
+  <si>
+    <t>RECENTLYVISITED</t>
   </si>
 </sst>
 </file>
@@ -512,13 +515,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB183B-02B6-F140-9F88-75932E878015}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -905,8 +910,85 @@
       <c r="I24" s="7"/>
       <c r="J24" s="5"/>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="B12:B14"/>

</xml_diff>

<commit_message>
update booking control flow excel
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonqiu/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyicui/Documents/GitHub/Dulwich Bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A156F4DA-C0B7-994D-8823-E6711BC8795C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3163E32-6F96-E947-AF46-005EF2469953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1820" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
+    <workbookView xWindow="9500" yWindow="1840" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="20">
   <si>
     <t>DELETE 1</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>BOOKMARK</t>
+  </si>
+  <si>
+    <t>RECENTLYVISITED</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -199,6 +202,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -515,9 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB183B-02B6-F140-9F88-75932E878015}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -984,8 +993,85 @@
       <c r="I29" s="7"/>
       <c r="J29" s="5"/>
     </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B32:B34"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B7:B9"/>

</xml_diff>

<commit_message>
update access control flow excel
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyicui/Documents/GitHub/Dulwich Bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3163E32-6F96-E947-AF46-005EF2469953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2DF713-7680-1D40-A101-D3C9696C266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9500" yWindow="1840" windowWidth="28040" windowHeight="17440" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="21">
   <si>
     <t>DELETE 1</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>RECENTLYVISITED</t>
+  </si>
+  <si>
+    <t>TAGMAP</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -188,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -201,13 +210,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB183B-02B6-F140-9F88-75932E878015}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,7 +585,7 @@
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="5"/>
@@ -589,7 +601,7 @@
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
       <c r="E3" s="5"/>
@@ -603,7 +615,7 @@
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -649,7 +661,7 @@
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="6"/>
@@ -665,7 +677,7 @@
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
@@ -679,7 +691,7 @@
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -725,7 +737,7 @@
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="6"/>
@@ -741,7 +753,7 @@
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -755,7 +767,7 @@
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="8"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -801,7 +813,7 @@
       <c r="A17" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="6"/>
@@ -817,7 +829,7 @@
       <c r="A18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -831,7 +843,7 @@
       <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -877,7 +889,7 @@
       <c r="A22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C22" s="6"/>
@@ -893,7 +905,7 @@
       <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -907,7 +919,7 @@
       <c r="A24" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -953,12 +965,12 @@
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="5"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
@@ -969,10 +981,10 @@
       <c r="A28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="5"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -983,10 +995,10 @@
       <c r="A29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="5"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -1026,15 +1038,15 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="E32" s="11"/>
       <c r="F32" s="5"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
@@ -1042,13 +1054,13 @@
       <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="10"/>
+      <c r="B33" s="9"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="5"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
@@ -1056,21 +1068,98 @@
       <c r="J33" s="5"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="10"/>
+      <c r="B34" s="9"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="5"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="5"/>
     </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B37:B39"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="B2:B4"/>

</xml_diff>

<commit_message>
Update access control flow with resourceBooking
</commit_message>
<xml_diff>
--- a/docs/DULWICH BOOKINGS Access Control Flow.xlsx
+++ b/docs/DULWICH BOOKINGS Access Control Flow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shenyicui/Documents/GitHub/Dulwich Bookings/Dulwich-Bookings-API/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonqiu/Desktop/dulwich-bookings/Dulwich-Bookings-API/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B91289-AA95-894C-A9AF-E591EE8BBCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711CB542-9FB7-0243-AF63-4DF694FABE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{242A94BE-306E-A54E-B2EA-82EE4BD064D4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="24">
   <si>
     <t>DELETE 1</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>MILESTONE</t>
+  </si>
+  <si>
+    <t>RESOURCEBOOKING</t>
   </si>
 </sst>
 </file>
@@ -540,15 +543,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB183B-02B6-F140-9F88-75932E878015}">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1315,18 +1318,95 @@
       <c r="I49" s="7"/>
       <c r="J49" s="5"/>
     </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="12"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="12"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B22:B24"/>
     <mergeCell ref="B47:B49"/>
     <mergeCell ref="B42:B44"/>
     <mergeCell ref="B37:B39"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B22:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>